<commit_message>
Final Upload of All Relevant Documents
</commit_message>
<xml_diff>
--- a/Product Backlog.xlsx
+++ b/Product Backlog.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -535,7 +536,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="H20" activeCellId="1" sqref="A17 H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>